<commit_message>
Continuar con cambios en SQL
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -16,10 +16,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -33,7 +41,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -41,12 +49,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,14 +438,257 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>task_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>prompt</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>canonical_solution</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>test_sql/0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>How many products do we have? | products : product_id, country, price</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>['SELECT COUNT(*) FROM PRODUCTS']</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[False]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test_sql/1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>What is the total number of orders? | orders : order_id, description</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['SELECT COUNT(*) FROM ORDERS']</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[False]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>test_sql/2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>What is the average , minimum , and maximum price of all Spanish products? | products : product_id, country, price</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>["SELECT AVG(PRICE), MIN(PRICE), MAX(PRICE) FROM PRODUCTS WHERE COUNTRY = 'SPAIN'"]</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[False]</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>test_sql/3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Show all countries and the number of products in each country | products</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['SELECT COUNTRY, COUNT(*) FROM PRODUCTS GROUP BY COUNTRY']</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[False]</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>test_sql/4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>How many sales are there in store STORE1? | sales: sale_id, product_id, customer_id, quantity, store</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>["SELECT STORE, COUNT(*) FROM SALES WHERE BY STORE = 'STORE1'"]</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>[False]</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>test_sql/5</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>List all names by customers above the average age | customers: customer_id, name, surname, age</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['SELECT NAME FROM CUSTOMERS WHERE AGE &gt; (SELECT AVG(AGE) FROM CUSTOMERS)']</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>[False]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>test_sql/6</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>How many orders have products that their prices sum up to 100 or more? | sales: sale_id, product_id, customer_id, quantity, store | orders : order_id, description | order_product : order_id, product_id, price | products : product_id, country, price</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['SELECT COUNT(*) FROM ORDERS AS T1 JOIN ORDER_PRODUCT AS T2 ON T1.ORDER_ID = T2.ORDER_ID WHERE T2.PRICE &gt;= 100']</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>[False]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>test_sql/7</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>For all sales , what is the most frequent store? | sales: sale_id, product_id, customer_id, quantity, store</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['SELECT STORE, COUNT(STORE) FROM SALES GROUP BY STORE ORDER BY COUNT(STORE) DESC LIMIT 1']</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>[False]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>test_sql/8</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Show the sale that has the spanish product with higher quantity | sales: sale_id, product_id, customer_id, quantity, store |  orders : order_id, description | order_product : order_id, product_id, price | products : product_id, country, price</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>["SELECT T1.SALE_ID FROM SALES AS T1 JOIN ORDER_PRODUCT AS T2 ON T1.PRODUCT_ID = T2.PRODUCT_ID WHERE T2.COUNTRY = 'SPAIN' AND T1.QUANTITY &gt; 1"]</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>[False]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>test_sql/9</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Who is the customer that has more sales than the rest? | sales: sale_id, product_id, customer_id, quantity, store | customers: customer_id, name, surname, age</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[' SELECT NAME FROM CUSTOMERS AS T1 JOIN SALES AS T2 ON T1.CUSTOMER_ID = T2.CUSTOMER_ID GROUP BY T1.CUSTOMER_ID ORDER BY SUM(T2.SALES_ID) DESC LIMIT 1']</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>[False]</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uso de arquitectura con modelo CodeGPT
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,17 +471,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>test_sql/0</t>
+          <t>test/0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>How many products do we have? | products : product_id, country, price</t>
+          <t xml:space="preserve">
+def incr_list(l: list):
+    """Return list with elements incremented by 1.
+    &gt;&gt;&gt; incr_list([1, 2, 3])
+    [2, 3, 4]
+    &gt;&gt;&gt; incr_list([5, 3, 5, 2, 3, 3, 9, 0, 123])
+    [6, 4, 6, 3, 4, 4, 10, 1, 124]
+    """
+</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['select count(*) from products']</t>
+          <t>['\n\ndef incr_list(l: list):\n    """Return list with elements incremented by 1.\n    &gt;&gt;&gt; incr_list([1, 2, 3])\n    [2, 3, 4]\n    &gt;&gt;&gt; incr_list([5, 3, 5, 2, 3, 3, 9, 0, 123])\n    [6, 4, 6, 3, 4, 4, 10, 1, 124]\n    """\n_list = [] for i in range(len(l)): if l[i] == \'y\': # y is a bit of a bit of a bit of a # bit of a character. # y is a bit of a character. # y is a bit of a character. # y is a bit of a character. # y is a bit of a character. # y is a bit of a character. # y is a bit of a character']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -493,17 +501,35 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>test_sql/1</t>
+          <t>test/1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>What is the total number of orders? | orders : order_id, description</t>
+          <t xml:space="preserve">
+def is_prime(n):
+    """Return true if a given number is prime, and false otherwise.
+    &gt;&gt;&gt; is_prime(6)
+    False
+    &gt;&gt;&gt; is_prime(101)
+    True
+    &gt;&gt;&gt; is_prime(11)
+    True
+    &gt;&gt;&gt; is_prime(13441)
+    True
+    &gt;&gt;&gt; is_prime(61)
+    True
+    &gt;&gt;&gt; is_prime(4)
+    False
+    &gt;&gt;&gt; is_prime(1)
+    False
+    """
+</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['select count(*) from orders']</t>
+          <t>['\n\ndef is_prime(n):\n    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n = True # True means \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'']</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -515,17 +541,29 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>test_sql/2</t>
+          <t>test/2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>What is the average , minimum , and maximum price of all spanish products? | products : product_id, country, price</t>
+          <t xml:space="preserve">
+def add_elements(arr, k):
+    """
+    Given a non-empty array of integers arr and an integer k, return
+    the sum of the elements with at most two digits from the first k elements of arr.
+    Example:
+        Input: arr = [111,21,3,4000,5,6,7,8,9], k = 4
+        Output: 24 # sum of 21 + 3
+    Constraints:
+        1. 1 &lt;= len(arr) &lt;= 100
+        2. 1 &lt;= k &lt;= len(arr)
+    """
+</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>["select avg(price), min(price), max(price) from products where counstry = 'SPAIN'"]</t>
+          <t>['\ndef add_elements(arr, k):\n    """\n    Given a non-empty array of integers arr and an integer k, return\n    the sum of the elements with at most two digits from the first k elements of arr.\n\n    Example:\n\n        Input: arr = [111,21,3,4000,5,6,7,8,9], k = 4\n        Output: 24 # sum of 21 + 3\n\n    Constraints:\n        1. 1 &lt;= len(arr) &lt;= 100\n        2. 1 &lt;= k &lt;= len(arr)\n    """\n 负ary orhood orhood orhood orhood orhood orhood orhood orhood orhood orhood or']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -537,17 +575,25 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>test_sql/3</t>
+          <t>test/3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Show all countries and the number of products in each country | products</t>
+          <t xml:space="preserve">
+def solution(lst):
+    """Given a non-empty list of integers, return the sum of all of the odd elements that are in even positions.
+    Examples
+    solution([5, 8, 7, 1]) ==&gt; 12
+    solution([3, 3, 3, 3, 3]) ==&gt; 9
+    solution([30, 13, 24, 321]) ==&gt;0
+    """
+</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['select country, count(*) from products group by country']</t>
+          <t>['\ndef solution(lst):\n    """Given a non-empty list of integers, return the sum of all of the odd elements that are in even positions.\n    \n\n    Examples\n    solution([5, 8, 7, 1]) ==&gt; 12\n    solution([3, 3, 3, 3, 3]) ==&gt; 9\n    solution([30, 13, 24, 321]) ==&gt;0\n    """\n = 0 for index, piece in enumerate(lst): if piece == cardinal: cardinal = index return cardinal ']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -559,130 +605,29 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>test_sql/4</t>
+          <t>test/4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>How many sales are there in store STORE1? | sales: sale_id, product_id, customer_id, quantity, store</t>
+          <t xml:space="preserve">
+def digits(n):
+    """Given a positive integer n, return the product of the odd digits.
+    Return 0 if all digits are even.
+    For example:
+    digits(1)  == 1
+    digits(4)  == 0
+    digits(235) == 15
+    """
+</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>["select store, count(*) from sales where store = 'STORE1'"]</t>
+          <t>['\ndef digits(n):\n    """Given a positive integer n, return the product of the odd digits.\n    Return 0 if all digits are even.\n    For example:\n    digits(1)  == 1\n    digits(4)  == 0\n    digits(235) == 15\n    """\n 度 """ if n % 2 == 0: return 0 if n % 2 == 1: return 1 if n % 2 == 2: return 2 if n % 2 == 0: return 2 if n % 2 == 0: return 3 if n % 2 == 0: return 4 if n % 2 == 0: return 4 if n % 2 == 0: return 4 if n % 2 == 0: return 4 ']</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>[True]</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>test_sql/5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>List all names by customers above the average age | customers: customer_id, name, surname, age</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>['select name from customers where age &gt; (select avg(age) from customers)']</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>[True]</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>test_sql/6</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>How many orders have products that their prices sum up to 100 or more? | sales: sale_id, product_id, customer_id, quantity, store | orders : order_id, description | order_product : order_id, product_id, price | products : product_id, country, price</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>['select count(*) from orders as t1 join order_product as t2 on t1.order_id = t2.order_id where t2.price &gt;= 100']</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>[True]</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>test_sql/7</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>For all sales , what is the most frequent store? | sales: sale_id, product_id, customer_id, quantity, store</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>['select store, count(store) from sales group by store order by count(store) desc limit 1']</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>[True]</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>test_sql/8</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Show the sale that has the spanish product with higher quantity | sales: sale_id, product_id, customer_id, quantity, store |  orders : order_id, description | order_product : order_id, product_id, price | products : product_id, country, price</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>["select t1.sale_id from sales as t1 join order_product as t2 on t1.product_id = t2.product_id where t2.country = 'SPAIN' and t1.quantity &gt; 1"]</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>[False]</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>test_sql/9</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Who is the customer that has more sales than the rest? | sales: sale_id, product_id, customer_id, quantity, store | customers: customer_id, name, surname, age</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>['select name from customers as t1 join sales as t2 on t1.customer_id = t2.customer_id group by t1.customer_id order by sum(t2.sales_id) desc limit 1']</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
         <is>
           <t>[False]</t>
         </is>

</xml_diff>

<commit_message>
Adaptación de problemas al modelo GPT Neo y nueva clase de Unit Testing
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -1,12 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -25,12 +26,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -50,19 +46,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -75,7 +62,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -438,9 +425,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -454,15 +441,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>question</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>prompt</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>canonical_solution</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>result</t>
         </is>
@@ -476,9 +468,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-def incr_list(l: list):
-    """Return list with elements incremented by 1.
+          <t xml:space="preserve">"""Return list with elements incremented by 1.
     &gt;&gt;&gt; incr_list([1, 2, 3])
     [2, 3, 4]
     &gt;&gt;&gt; incr_list([5, 3, 5, 2, 3, 3, 9, 0, 123])
@@ -489,10 +479,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['\n\ndef incr_list(l: list):\n    """Return list with elements incremented by 1.\n    &gt;&gt;&gt; incr_list([1, 2, 3])\n    [2, 3, 4]\n    &gt;&gt;&gt; incr_list([5, 3, 5, 2, 3, 3, 9, 0, 123])\n    [6, 4, 6, 3, 4, 4, 10, 1, 124]\n    """\n_list = [] for i in range(len(l)): if l[i] == \'y\': # y is a bit of a bit of a bit of a # bit of a character. # y is a bit of a character. # y is a bit of a character. # y is a bit of a character. # y is a bit of a character. # y is a bit of a character. # y is a bit of a character']</t>
+          <t xml:space="preserve">
+def incr_list(l: list):
+</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
+        <is>
+          <t>['\nQUESTION:\n\n\ndef incr_list(l: list):\n\n\n\ndef incr_list(l: list):\n\n\nUse Call-Based Format\n\nANSWER:\ndef incr_list(l):\n\treturn list(map(lambda x,y: x+y, l))\n&lt;|endoftext|&gt;']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>[True]</t>
         </is>
@@ -506,9 +503,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-def is_prime(n):
-    """Return true if a given number is prime, and false otherwise.
+          <t xml:space="preserve">"""Return true if a given number is prime, and false otherwise.
     &gt;&gt;&gt; is_prime(6)
     False
     &gt;&gt;&gt; is_prime(101)
@@ -529,10 +524,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['\n\ndef is_prime(n):\n    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n = True # True means \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'xxx\' == \'']</t>
+          <t xml:space="preserve">
+def is_prime(n):
+</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>['\nQUESTION:\n\n\ndef is_prime(n):\n\n\n\ndef is_prime(n):\n\n\nUse Call-Based Format\n\nANSWER:\nimport math\ndef is_prime(n):\n\tif n &lt; 2:\n\t\treturn False\n\tfor i in range(2, int(math.sqrt(n)) + 1):\n\t\tif n % i == 0:\n\t\t\treturn False\n\treturn True\n&lt;|endoftext|&gt;']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>[True]</t>
         </is>
@@ -546,9 +548,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-def add_elements(arr, k):
-    """
+          <t xml:space="preserve">"""
     Given a non-empty array of integers arr and an integer k, return
     the sum of the elements with at most two digits from the first k elements of arr.
     Example:
@@ -563,12 +563,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['\ndef add_elements(arr, k):\n    """\n    Given a non-empty array of integers arr and an integer k, return\n    the sum of the elements with at most two digits from the first k elements of arr.\n\n    Example:\n\n        Input: arr = [111,21,3,4000,5,6,7,8,9], k = 4\n        Output: 24 # sum of 21 + 3\n\n    Constraints:\n        1. 1 &lt;= len(arr) &lt;= 100\n        2. 1 &lt;= k &lt;= len(arr)\n    """\n 负ary orhood orhood orhood orhood orhood orhood orhood orhood orhood orhood or']</t>
+          <t xml:space="preserve">
+def add_elements(arr, k):
+</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[False]</t>
+          <t>['\nQUESTION:\n\ndef add_elements(arr, k):\n\n\ndef add_elements(arr, k):\n\n\nUse Call-Based Format\n\nANSWER:\ndef add_elements(arr, k):\n\tarr.append(k)\n\treturn arr\n&lt;|endoftext|&gt;']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[True]</t>
         </is>
       </c>
     </row>
@@ -580,9 +587,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-def solution(lst):
-    """Given a non-empty list of integers, return the sum of all of the odd elements that are in even positions.
+          <t xml:space="preserve">"""Given a non-empty list of integers, return the sum of all of the odd elements that are in even positions.
     Examples
     solution([5, 8, 7, 1]) ==&gt; 12
     solution([3, 3, 3, 3, 3]) ==&gt; 9
@@ -593,10 +598,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['\ndef solution(lst):\n    """Given a non-empty list of integers, return the sum of all of the odd elements that are in even positions.\n    \n\n    Examples\n    solution([5, 8, 7, 1]) ==&gt; 12\n    solution([3, 3, 3, 3, 3]) ==&gt; 9\n    solution([30, 13, 24, 321]) ==&gt;0\n    """\n = 0 for index, piece in enumerate(lst): if piece == cardinal: cardinal = index return cardinal ']</t>
+          <t xml:space="preserve">
+def solution(lst):
+</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
+        <is>
+          <t>['\nQUESTION:\n\ndef solution(lst):\n\n\ndef solution(lst):\n\n\nUse Call-Based Format\n\nANSWER:\ndef solution(lst):\n\treturn sum(lst)/len(lst)\n&lt;|endoftext|&gt;']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>[True]</t>
         </is>
@@ -610,9 +622,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-def digits(n):
-    """Given a positive integer n, return the product of the odd digits.
+          <t xml:space="preserve">"""Given a positive integer n, return the product of the odd digits.
     Return 0 if all digits are even.
     For example:
     digits(1)  == 1
@@ -624,16 +634,23 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['\ndef digits(n):\n    """Given a positive integer n, return the product of the odd digits.\n    Return 0 if all digits are even.\n    For example:\n    digits(1)  == 1\n    digits(4)  == 0\n    digits(235) == 15\n    """\n 度 """ if n % 2 == 0: return 0 if n % 2 == 1: return 1 if n % 2 == 2: return 2 if n % 2 == 0: return 2 if n % 2 == 0: return 3 if n % 2 == 0: return 4 if n % 2 == 0: return 4 if n % 2 == 0: return 4 if n % 2 == 0: return 4 ']</t>
+          <t xml:space="preserve">
+def digits(n):
+</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[False]</t>
+          <t>['\nQUESTION:\n\ndef digits(n):\n\n\ndef digits(n):\n\n\nUse Call-Based Format\n\nANSWER:\ndef digits(n):\n\treturn [int(x) for x in str(n)]\n&lt;|endoftext|&gt;']</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>[True]</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adaptación de la arquitectura al modelo Codex
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['\nQUESTION:\n\n\ndef incr_list(l: list):\n\n\n\ndef incr_list(l: list):\n\n\nUse Call-Based Format\n\nANSWER:\ndef incr_list(l):\n\treturn list(map(lambda x,y: x+y, l))\n&lt;|endoftext|&gt;']</t>
+          <t>['    return [x + 1 for x in l]\n\n\ndef main():\n    """Run program and print function docstrings."""\n    print(__doc__)\n    print(incr_list.__doc__)\n\n\nif __name__ == "__main__":\n    main()']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -531,7 +531,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['\nQUESTION:\n\n\ndef is_prime(n):\n\n\n\ndef is_prime(n):\n\n\nUse Call-Based Format\n\nANSWER:\nimport math\ndef is_prime(n):\n\tif n &lt; 2:\n\t\treturn False\n\tfor i in range(2, int(math.sqrt(n)) + 1):\n\t\tif n % i == 0:\n\t\t\treturn False\n\treturn True\n&lt;|endoftext|&gt;']</t>
+          <t>['    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n    if n == 1:\n        return False\n    elif n == 2:\n        return True\n    else:\n        for i in range(2, n):\n            if n % i == 0:\n                return False\n        return True\n\n\ndef is_prime(n):\n    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n    if n == 1:\n        return False\n    elif n == 2:\n        return True\n    else:\n        for i in range(2, n):\n            if n % i == 0:\n                return False\n        return True\n\n\ndef is_prime(n):\n    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n    if n == 1:\n        return False\n    elif n == 2:\n        return True\n    else:\n        for i in range(2, n):\n            if n % i == 0:\n                return False\n        return True\n\n\ndef is_prime(n):\n    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n    if n == 1:\n        return False\n    elif n == 2:\n        return True\n    else:\n        for i in range(2, n):\n            if n % i == 0:\n                return False\n        return True\n\n\ndef is_prime(n):\n    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n    if n == 1:\n        return False\n    elif n == 2:\n        return True\n    else:\n        for i in range(2, n):\n            if n % i == 0:\n                return False\n        return True\n\n\ndef is_prime(n):\n    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n    if n == 1:\n        return False\n    elif n == 2:\n        return True\n    else:\n        for i in range(2, n):\n            if n % i == 0:\n                return False\n        return True\n\n\ndef is_prime(n):\n    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n    if n == 1:\n        return False\n    elif n == 2:\n        return True\n    else:\n        for i in range(2, n):\n            if n % i == 0:\n                return False\n        return True\n\n\ndef is_prime(n):\n    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n    if n == 1:\n        return False\n    elif n == 2:\n        return True\n    else:\n        for i in range(2, n):\n            if n % i == 0:\n                return False\n        return True\n\n\ndef is_prime(n):\n    """Return true if a given number is prime, and false otherwise.\n    &gt;&gt;&gt; is_prime(6)\n    False\n    &gt;&gt;&gt; is_prime(101)\n    True\n    &gt;&gt;&gt; is_prime(11)\n    True\n    &gt;&gt;&gt; is_prime(13441)\n    True\n    &gt;&gt;&gt; is_prime(61)\n    True\n    &gt;&gt;&gt; is_prime(4)\n    False\n    &gt;&gt;&gt; is_prime(1)\n    False\n    """\n    if n == 1:\n        return False\n    elif n == 2:\n        return True\n    else:\n        for i in range(2, n):\n            if n % i == 0:\n                return False\n']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -570,7 +570,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['\nQUESTION:\n\ndef add_elements(arr, k):\n\n\ndef add_elements(arr, k):\n\n\nUse Call-Based Format\n\nANSWER:\ndef add_elements(arr, k):\n\tarr.append(k)\n\treturn arr\n&lt;|endoftext|&gt;']</t>
+          <t>['    """\n    Time Complexity: O(n)\n    Space Complexity: O(1)\n    """\n    total = 0\n    for i in range(k):\n        if arr[i] &lt; 10:\n            total += arr[i]\n        elif arr[i] &lt; 100:\n            total += arr[i] % 10 + arr[i] // 10\n    return total\n\nif __name__ == "__main__":\n    arr = [111,21,3,4000,5,6,7,8,9]\n    k = 4\n    print(add_elements(arr, k))']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['\nQUESTION:\n\ndef solution(lst):\n\n\ndef solution(lst):\n\n\nUse Call-Based Format\n\nANSWER:\ndef solution(lst):\n\treturn sum(lst)/len(lst)\n&lt;|endoftext|&gt;']</t>
+          <t>['    return sum(lst[i] for i in range(1, len(lst), 2) if lst[i] % 2 == 1)\n\nprint(solution([5, 8, 7, 1]))\nprint(solution([3, 3, 3, 3, 3]))\nprint(solution([30, 13, 24, 321]))']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['\nQUESTION:\n\ndef digits(n):\n\n\ndef digits(n):\n\n\nUse Call-Based Format\n\nANSWER:\ndef digits(n):\n\treturn [int(x) for x in str(n)]\n&lt;|endoftext|&gt;']</t>
+          <t>['    return reduce(lambda x, y: x * y, [int(i) for i in str(n) if int(i) % 2 != 0])\n\nprint(digits(1))\nprint(digits(4))\nprint(digits(235))']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">

</xml_diff>